<commit_message>
twin weights and L8 quiz histograms update
</commit_message>
<xml_diff>
--- a/docs/Data/TwinWeights.xlsx
+++ b/docs/Data/TwinWeights.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://webmailbyui-my.sharepoint.com/personal/drp36_byui_edu/Documents/221/Course_Files/BYUI_M221_Book/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://webmailbyui-my.sharepoint.com/personal/drp36_byui_edu/Documents/221/Course_Files/BYUI_M221_Book/docs/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1795,16 +1795,16 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC863457-4CFF-4F01-AD02-A883A629F113}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="1c0769b7-2dc5-4346-9277-bf71cefdc793"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="56caf978-ed08-4319-8660-ea565c3c81d4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="1c0769b7-2dc5-4346-9277-bf71cefdc793"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>